<commit_message>
add prediction exp, add test pred config on train, make mixing switchable
</commit_message>
<xml_diff>
--- a/receptive_field.xlsx
+++ b/receptive_field.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\audio_tagging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BC73E9-C273-44CF-B9A1-1CE820F9D1C2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B8A859-1D02-48A6-B4E8-1A48C4B70435}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0C91D080-4855-489F-A6D3-86FC3CD1DB13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0C91D080-4855-489F-A6D3-86FC3CD1DB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +995,7 @@
         <v>60</v>
       </c>
       <c r="C15">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="D15">
         <v>80</v>
@@ -1019,12 +1019,12 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <f>(B15-E15+2*I15)/G15+1</f>
+        <f t="shared" ref="K15:L18" si="16">(B15-E15+2*I15)/G15+1</f>
         <v>4</v>
       </c>
       <c r="L15">
-        <f>(C15-F15+2*J15)/H15+1</f>
-        <v>36</v>
+        <f t="shared" si="16"/>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1032,12 +1032,12 @@
         <v>24</v>
       </c>
       <c r="B16">
-        <f>K15</f>
+        <f t="shared" ref="B16:C18" si="17">K15</f>
         <v>4</v>
       </c>
       <c r="C16">
-        <f>L15</f>
-        <v>36</v>
+        <f t="shared" si="17"/>
+        <v>72</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1061,12 +1061,12 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <f>(B16-E16+2*I16)/G16+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="L16">
-        <f>(C16-F16+2*J16)/H16+1</f>
-        <v>12</v>
+        <f t="shared" si="16"/>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1074,12 +1074,12 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <f>K16</f>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="C17">
-        <f>L16</f>
-        <v>12</v>
+        <f t="shared" si="17"/>
+        <v>24</v>
       </c>
       <c r="D17">
         <v>80</v>
@@ -1103,12 +1103,12 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <f>(B17-E17+2*I17)/G17+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="L17">
-        <f>(C17-F17+2*J17)/H17+1</f>
-        <v>9</v>
+        <f t="shared" si="16"/>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -1116,12 +1116,12 @@
         <v>24</v>
       </c>
       <c r="B18">
-        <f>K17</f>
+        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="C18">
-        <f>L17</f>
-        <v>9</v>
+        <f t="shared" si="17"/>
+        <v>21</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1145,12 +1145,12 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <f>(B18-E18+2*I18)/G18+1</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="L18">
-        <f>(C18-F18+2*J18)/H18+1</f>
-        <v>3</v>
+        <f t="shared" si="16"/>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>